<commit_message>
INSERIDO EXAME PROSTATA JULIANE ARRUDA
</commit_message>
<xml_diff>
--- a/colaborador/sistemas/orcamento/valores_exames_samvida.xlsx
+++ b/colaborador/sistemas/orcamento/valores_exames_samvida.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="489">
   <si>
     <t>Local</t>
   </si>
@@ -1211,7 +1211,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1237,7 +1236,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dra. JULIANA)</t>
@@ -1254,7 +1252,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dra. JULIANA)</t>
@@ -1271,7 +1268,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1294,7 +1290,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1311,7 +1306,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dra, JULIANA)</t>
@@ -1328,7 +1322,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dra, JULIANA)</t>
@@ -1351,7 +1344,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1368,7 +1360,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1385,7 +1376,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1414,7 +1404,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="64"/>
         <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">(Dr. JOSE GERALDO)</t>
@@ -1617,6 +1606,12 @@
   </si>
   <si>
     <t xml:space="preserve">COLPOSCOPIA (Dr. MOARCY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USG PROSTATA (Dra. JULIANE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USG PROSTATA C/ DOPPLER (Dra. JULIANE)</t>
   </si>
   <si>
     <t xml:space="preserve">PAAF - NODULO ADICIONAL R$ 100,00 (Dra. JULIANE)</t>
@@ -1635,19 +1630,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1672,7 +1662,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="64"/>
+        <fgColor indexed="58"/>
         <bgColor indexed="58"/>
       </patternFill>
     </fill>
@@ -1711,24 +1701,24 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="4" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1746,10 +1736,6 @@
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -6746,7 +6732,7 @@
       <c r="A410" t="s">
         <v>52</v>
       </c>
-      <c r="B410" s="10" t="s">
+      <c r="B410" s="8" t="s">
         <v>412</v>
       </c>
       <c r="C410" s="2">
@@ -6757,7 +6743,7 @@
       <c r="A411" t="s">
         <v>52</v>
       </c>
-      <c r="B411" s="10" t="s">
+      <c r="B411" s="8" t="s">
         <v>413</v>
       </c>
       <c r="C411" s="2">
@@ -7512,7 +7498,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="480" ht="14.25">
+    <row r="480" ht="13.800000000000001">
       <c r="A480" t="s">
         <v>52</v>
       </c>
@@ -7520,10 +7506,10 @@
         <v>483</v>
       </c>
       <c r="C480" s="2">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="481" ht="14.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="481" ht="13.800000000000001">
       <c r="A481" t="s">
         <v>52</v>
       </c>
@@ -7531,10 +7517,10 @@
         <v>484</v>
       </c>
       <c r="C481" s="2">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="482" ht="13.800000000000001">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="482" ht="14.25">
       <c r="A482" t="s">
         <v>52</v>
       </c>
@@ -7542,10 +7528,10 @@
         <v>485</v>
       </c>
       <c r="C482" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="483" ht="13.800000000000001">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="483" ht="14.25">
       <c r="A483" t="s">
         <v>52</v>
       </c>
@@ -7553,21 +7539,43 @@
         <v>486</v>
       </c>
       <c r="C483" s="2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="484" ht="13.800000000000001">
+      <c r="A484" t="s">
+        <v>52</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C484" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="485" ht="13.800000000000001">
+      <c r="A485" t="s">
+        <v>52</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C485" s="2">
         <v>185</v>
       </c>
     </row>
-    <row r="1048266" ht="12.800000000000001"/>
-    <row r="1048267" ht="12.800000000000001"/>
     <row r="1048268" ht="12.800000000000001"/>
     <row r="1048269" ht="12.800000000000001"/>
-    <row r="1048567" ht="12.800000000000001"/>
-    <row r="1048568" ht="12.800000000000001"/>
+    <row r="1048270" ht="12.800000000000001"/>
+    <row r="1048271" ht="12.800000000000001"/>
     <row r="1048569" ht="12.800000000000001"/>
     <row r="1048570" ht="12.800000000000001"/>
     <row r="1048571" ht="12.800000000000001"/>
     <row r="1048572" ht="12.800000000000001"/>
     <row r="1048573" ht="12.800000000000001"/>
     <row r="1048574" ht="12.800000000000001"/>
+    <row r="1048575" ht="12.800000000000001"/>
+    <row r="1048576" ht="12.800000000000001"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51181102362204689" footer="0.51181102362204689"/>

</xml_diff>

<commit_message>
INSERIDO EXAME VULVOSCOPIA MOARCY
</commit_message>
<xml_diff>
--- a/colaborador/sistemas/orcamento/valores_exames_samvida.xlsx
+++ b/colaborador/sistemas/orcamento/valores_exames_samvida.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="490">
   <si>
     <t>Local</t>
   </si>
@@ -1603,6 +1603,9 @@
   </si>
   <si>
     <t xml:space="preserve">USG VASOS CERVICAIS (Dr. MOARCY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VULVOSCOPIA (Dr. MOARCY)</t>
   </si>
   <si>
     <t xml:space="preserve">COLPOSCOPIA (Dr. MOARCY)</t>
@@ -2218,7 +2221,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="A384" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="A460" zoomScale="100" workbookViewId="0">
       <selection activeCell="B485" activeCellId="0" sqref="B485"/>
     </sheetView>
   </sheetViews>
@@ -7500,13 +7503,13 @@
     </row>
     <row r="480" ht="13.800000000000001">
       <c r="A480" t="s">
-        <v>52</v>
+        <v>430</v>
       </c>
       <c r="B480" s="1" t="s">
         <v>483</v>
       </c>
       <c r="C480" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="481" ht="13.800000000000001">
@@ -7517,10 +7520,10 @@
         <v>484</v>
       </c>
       <c r="C481" s="2">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="482" ht="14.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="482" ht="13.800000000000001">
       <c r="A482" t="s">
         <v>52</v>
       </c>
@@ -7528,7 +7531,7 @@
         <v>485</v>
       </c>
       <c r="C482" s="2">
-        <v>210</v>
+        <v>160</v>
       </c>
     </row>
     <row r="483" ht="14.25">
@@ -7539,10 +7542,10 @@
         <v>486</v>
       </c>
       <c r="C483" s="2">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="484" ht="13.800000000000001">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="484" ht="14.25">
       <c r="A484" t="s">
         <v>52</v>
       </c>
@@ -7550,7 +7553,7 @@
         <v>487</v>
       </c>
       <c r="C484" s="2">
-        <v>140</v>
+        <v>430</v>
       </c>
     </row>
     <row r="485" ht="13.800000000000001">
@@ -7561,14 +7564,24 @@
         <v>488</v>
       </c>
       <c r="C485" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="486" ht="13.800000000000001">
+      <c r="A486" t="s">
+        <v>52</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C486" s="2">
         <v>185</v>
       </c>
     </row>
-    <row r="1048268" ht="12.800000000000001"/>
     <row r="1048269" ht="12.800000000000001"/>
     <row r="1048270" ht="12.800000000000001"/>
     <row r="1048271" ht="12.800000000000001"/>
-    <row r="1048569" ht="12.800000000000001"/>
+    <row r="1048272" ht="12.800000000000001"/>
     <row r="1048570" ht="12.800000000000001"/>
     <row r="1048571" ht="12.800000000000001"/>
     <row r="1048572" ht="12.800000000000001"/>

</xml_diff>